<commit_message>
final modification add: dockerignore
</commit_message>
<xml_diff>
--- a/work_dir/query_output.xlsx
+++ b/work_dir/query_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,96 +436,142 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>productLine</t>
+          <t>title</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>totalSales</t>
+          <t>tactic</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>technique</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>other_info</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Classic Cars</t>
+          <t>Antivirus Exploitation Framework Detection</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3853922.49</t>
+          <t>Execution</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>T1203</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Exploitation for Client Execution : Detecting exploitation of vulnerabilities for execution.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Motorcycles</t>
+          <t>Antivirus Hacktool Detection</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1121426.12</t>
+          <t>Execution</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>T1204.002</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>User Execution: Malicious File : Detection of tools requiring user execution to compromise systems.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Vintage Cars</t>
+          <t>Antivirus Password Dumper Detection</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1797559.63</t>
+          <t>Credential Access</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>T1003</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>OS Credential Dumping : Detecting tools attempting to dump OS credentials from memory.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Planes</t>
+          <t>Antivirus PrinterNightmare CVE-2021-34527 Exploit Detection</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>954637.54</t>
+          <t>Privilege Escalation</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>T1068</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Exploitation for Privilege Escalation : Detection of PrinterNightmare (CVE-2021-34527) exploit for privilege escalation.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Trucks and Buses</t>
+          <t>Antivirus Ransomware Detection</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1024113.57</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Ships</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>663998.34</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Trains</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>188532.92</t>
+          <t>Impact</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>T1486</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Data Encrypted for Impact : Detection of ransomware encrypting files to cause impact.</t>
         </is>
       </c>
     </row>

</xml_diff>